<commit_message>
change:update script to be compatible with linux and windows
</commit_message>
<xml_diff>
--- a/data/sample/benchmark_out.xlsx
+++ b/data/sample/benchmark_out.xlsx
@@ -1,37 +1,113 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coderush\code\3-SQL-Rewriter\data\sample\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2932856D-ED84-4510-B863-965FB1DBBBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+  <si>
+    <t>origin cost</t>
+  </si>
+  <si>
+    <t>rewrite cost</t>
+  </si>
+  <si>
+    <t>improvement</t>
+  </si>
+  <si>
+    <t>origin query</t>
+  </si>
+  <si>
+    <t>rewrite query</t>
+  </si>
+  <si>
+    <t>-16.55%</t>
+  </si>
+  <si>
+    <t>SELECT MIN(chn.name) AS uncredited_voiced_character, MIN(t.title) AS russian_movie FROM char_name AS chn, cast_info AS ci, company_name AS cn, company_type AS ct, movie_companies AS mc, role_type AS rt, title AS t WHERE ci.note LIKE '%(voice)%' AND ci.note LIKE '%(uncredited)%' AND cn.country_code = '[ru]' AND rt.role = 'actor' AND t.production_year &gt; 2005 AND t.id = mc.movie_id AND t.id = ci.movie_id AND ci.movie_id = mc.movie_id AND chn.id = ci.person_role_id AND rt.id = ci.role_id AND cn.id = mc.company_id AND ct.id = mc.company_type_id;</t>
+  </si>
+  <si>
+    <t>SELECT MIN(chn.name) AS uncredited_voiced_character, MIN(t.title) AS russian_movie FROM char_name AS chn, cast_info AS ci, company_name AS cn, company_type AS ct, movie_companies AS mc, role_type AS rt, title AS t WHERE ci.note LIKE '%(voice)%' AND ci.note LIKE '%(uncredited)%' AND cn.country_code = '[ru]' AND rt.role = 'actor' AND t.production_year &gt; 2005 AND t.id = mc.movie_id AND t.id = ci.movie_id AND ci.movie_id = mc.movie_id AND chn.id = ci.person_role_id AND rt.id = ci.role_id AND cn.id = mc.company_id AND ct.id = mc.company_type_id;;</t>
+  </si>
+  <si>
+    <t>SELECT MIN(chn.name) AS cname, MIN(t.title) AS russian_mov_with_actor_producer FROM char_name AS chn, cast_info AS ci, company_name AS cn, company_type AS ct, movie_companies AS mc, role_type AS rt, title AS t WHERE ci.note LIKE '%(producer)%' AND cn.country_code = '[ru]' AND rt.role = 'actor' AND t.production_year &gt; 2010 AND t.id = mc.movie_id AND t.id = ci.movie_id AND ci.movie_id = mc.movie_id AND chn.id = ci.person_role_id AND rt.id = ci.role_id AND cn.id = mc.company_id AND ct.id = mc.company_type_id;</t>
+  </si>
+  <si>
+    <t>SELECT MIN(chn.name) AS cname, MIN(t.title) AS russian_mov_with_actor_producer FROM char_name AS chn, cast_info AS ci, company_name AS cn, company_type AS ct, movie_companies AS mc, role_type AS rt, title AS t WHERE ci.note LIKE '%(producer)%' AND cn.country_code = '[ru]' AND rt.role = 'actor' AND t.production_year &gt; 2010 AND t.id = mc.movie_id AND t.id = ci.movie_id AND ci.movie_id = mc.movie_id AND chn.id = ci.person_role_id AND rt.id = ci.role_id AND cn.id = mc.company_id AND ct.id = mc.company_type_id;;</t>
+  </si>
+  <si>
+    <t>-1.82%</t>
+  </si>
+  <si>
+    <t>SELECT MIN(chn.name) AS cname, MIN(t.title) AS movie_with_american_producer FROM char_name AS chn, cast_info AS ci, company_name AS cn, company_type AS ct, movie_companies AS mc, role_type AS rt, title AS t WHERE ci.note LIKE '%(producer)%' AND cn.country_code = '[us]' AND t.production_year &gt; 1990 AND t.id = mc.movie_id AND t.id = ci.movie_id AND ci.movie_id = mc.movie_id AND chn.id = ci.person_role_id AND rt.id = ci.role_id AND cn.id = mc.company_id AND ct.id = mc.company_type_id;</t>
+  </si>
+  <si>
+    <t>SELECT MIN(chn.name) AS cname, MIN(t.title) AS movie_with_american_producer FROM char_name AS chn, cast_info AS ci, company_name AS cn, company_type AS ct, movie_companies AS mc, role_type AS rt, title AS t WHERE ci.note LIKE '%(producer)%' AND cn.country_code = '[us]' AND t.production_year &gt; 1990 AND t.id = mc.movie_id AND t.id = ci.movie_id AND ci.movie_id = mc.movie_id AND chn.id = ci.person_role_id AND rt.id = ci.role_id AND cn.id = mc.company_id AND ct.id = mc.company_type_id;;</t>
+  </si>
+  <si>
+    <t>-342.90%</t>
+  </si>
+  <si>
+    <t>SELECT MIN(cn.name) AS from_company, MIN(lt.link) AS movie_link_type, MIN(t.title) AS non_polish_sequel_movie FROM company_name AS cn, company_type AS ct, keyword AS k, link_type AS lt, movie_companies AS mc, movie_keyword AS mk, movie_link AS ml, title AS t WHERE cn.country_code !='[pl]' AND (cn.name LIKE '%Film%' OR cn.name LIKE '%Warner%') AND ct.kind ='production companies' AND k.keyword ='sequel' AND lt.link LIKE '%follow%' AND mc.note IS NULL AND t.production_year BETWEEN 1950 AND 2000 AND lt.id = ml.link_type_id AND ml.movie_id = t.id AND t.id = mk.movie_id AND mk.keyword_id = k.id AND t.id = mc.movie_id AND mc.company_type_id = ct.id AND mc.company_id = cn.id AND ml.movie_id = mk.movie_id AND ml.movie_id = mc.movie_id AND mk.movie_id = mc.movie_id;</t>
+  </si>
+  <si>
+    <t>SELECT MIN(cn.name) AS from_company, MIN(lt.link) AS movie_link_type, MIN(t.title) AS non_polish_sequel_movie FROM company_name AS cn, company_type AS ct, keyword AS k, link_type AS lt, movie_companies AS mc, movie_keyword AS mk, movie_link AS ml, title AS t WHERE cn.country_code !='[pl]' AND (cn.name LIKE '%Film%' OR cn.name LIKE '%Warner%') AND ct.kind ='production companies' AND k.keyword ='sequel' AND lt.link LIKE '%follow%' AND mc.note IS NULL AND t.production_year BETWEEN 1950 AND 2000 AND lt.id = ml.link_type_id AND ml.movie_id = t.id AND t.id = mk.movie_id AND mk.keyword_id = k.id AND t.id = mc.movie_id AND mc.company_type_id = ct.id AND mc.company_id = cn.id AND ml.movie_id = mk.movie_id AND ml.movie_id = mc.movie_id AND mk.movie_id = mc.movie_id;;</t>
+  </si>
+  <si>
+    <t>-347.34%</t>
+  </si>
+  <si>
+    <t>SELECT MIN(cn.name) AS from_company, MIN(lt.link) AS movie_link_type, MIN(t.title) AS sequel_movie FROM company_name AS cn, company_type AS ct, keyword AS k, link_type AS lt, movie_companies AS mc, movie_keyword AS mk, movie_link AS ml, title AS t WHERE cn.country_code !='[pl]' AND (cn.name LIKE '%Film%' OR cn.name LIKE '%Warner%') AND ct.kind ='production companies' AND k.keyword ='sequel' AND lt.link LIKE '%follows%' AND mc.note IS NULL AND t.production_year = 1998 AND t.title LIKE '%Money%' AND lt.id = ml.link_type_id AND ml.movie_id = t.id AND t.id = mk.movie_id AND mk.keyword_id = k.id AND t.id = mc.movie_id AND mc.company_type_id = ct.id AND mc.company_id = cn.id AND ml.movie_id = mk.movie_id AND ml.movie_id = mc.movie_id AND mk.movie_id = mc.movie_id;</t>
+  </si>
+  <si>
+    <t>SELECT MIN(cn.name) AS from_company, MIN(lt.link) AS movie_link_type, MIN(t.title) AS sequel_movie FROM company_name AS cn, company_type AS ct, keyword AS k, link_type AS lt, movie_companies AS mc, movie_keyword AS mk, movie_link AS ml, title AS t WHERE cn.country_code !='[pl]' AND (cn.name LIKE '%Film%' OR cn.name LIKE '%Warner%') AND ct.kind ='production companies' AND k.keyword ='sequel' AND lt.link LIKE '%follows%' AND mc.note IS NULL AND t.production_year = 1998 AND t.title LIKE '%Money%' AND lt.id = ml.link_type_id AND ml.movie_id = t.id AND t.id = mk.movie_id AND mk.keyword_id = k.id AND t.id = mc.movie_id AND mc.company_type_id = ct.id AND mc.company_id = cn.id AND ml.movie_id = mk.movie_id AND ml.movie_id = mc.movie_id AND mk.movie_id = mc.movie_id;;</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +122,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,93 +446,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.59765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>origin cost</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>rewrite cost</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>improvement</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>origin query</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>rewrite query</t>
-        </is>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1109709.26</v>
-      </c>
-      <c r="B2" t="n">
-        <v>4973265</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>-348.16%</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>SELECT MIN(mc.note) AS production_note, MIN(t.title) AS movie_title,        MIN(t.production_year) AS movie_year FROM company_type AS ct,      info_type AS it,      movie_companies AS mc,      movie_info_idx AS mi_idx,      title AS t WHERE ct.kind = 'production companies'   AND it.info = 'top 250 rank'   AND mc.note NOT LIKE '%(as Metro-Goldwyn-Mayer Pictures)%'   AND (mc.note LIKE '%(co-production)%'        OR mc.note LIKE '%(presents)%')   AND ct.id = mc.company_type_id   AND t.id = mc.movie_id   AND t.id = mi_idx.movie_id   AND mc.movie_id = mi_idx.movie_id   AND it.id = mi_idx.info_type_id;</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>SELECT MIN(`t103`.`production_note`) AS `production_note`, MIN(`t104`.`movie_title`) AS `movie_title`, MIN(`t104`.`movie_year`) AS `movie_year`  FROM (SELECT `t100`.`movie_id`, `t101`.`movie_id` AS `movie_id0`, MIN(`t100`.`production_note`) AS `production_note`  FROM (SELECT `t96`.`id` AS `id0`, `t98`.`movie_id`, MIN(`t98`.`production_note`) AS `production_note`  FROM (SELECT `id`  FROM `company_type`  WHERE `kind` = 'production companies'  GROUP BY `id`) AS `t94`,  (SELECT `id`  FROM `info_type`  WHERE `info` = 'top 250 rank'  GROUP BY `id`) AS `t96`,  (SELECT `movie_id`, `company_type_id`, MIN(`note`) AS `production_note`  FROM `movie_companies`  WHERE (`note` LIKE '%(co-production)%' OR `note` LIKE '%(presents)%') AND `note` NOT LIKE '%(as Metro-Goldwyn-Mayer Pictures)%'  GROUP BY `movie_id`, `company_type_id`) AS `t98`  WHERE `t94`.`id` = `t98`.`company_type_id`  GROUP BY `t96`.`id`, `t98`.`movie_id`) AS `t100`,  (SELECT `movie_id`, `info_type_id`  FROM `movie_info_idx`  GROUP BY `movie_id`, `info_type_id`) AS `t101`  WHERE `t100`.`movie_id` = `t101`.`movie_id` AND `t100`.`id0` = `t101`.`info_type_id`  GROUP BY `t100`.`movie_id`, `t101`.`movie_id`) AS `t103`,  (SELECT `id`, MIN(`title`) AS `movie_title`, MIN(`production_year`) AS `movie_year`  FROM `title`  GROUP BY `id`) AS `t104`  WHERE `t104`.`id` = `t103`.`movie_id` AND `t104`.`id` = `t103`.`movie_id0`;</t>
-        </is>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>215.1361057758331</v>
+      </c>
+      <c r="B2">
+        <v>250.75035548210141</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>817599.55</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1822932.29</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>-122.96%</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>SELECT MIN(mc.note) AS production_note,        MIN(t.title) AS movie_title,        MIN(t.production_year) AS movie_year FROM company_type AS ct,      info_type AS it,      movie_companies AS mc,      movie_info_idx AS mi_idx,      title AS t WHERE ct.kind = 'production companies'   AND it.info = 'bottom 10 rank'   AND mc.note NOT LIKE '%(as Metro-Goldwyn-Mayer Pictures)%'   AND t.production_year BETWEEN 2005 AND 2010   AND ct.id = mc.company_type_id   AND t.id = mc.movie_id   AND t.id = mi_idx.movie_id   AND mc.movie_id = mi_idx.movie_id   AND it.id = mi_idx.info_type_id;</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>SELECT MIN(`t609`.`production_note`) AS `production_note`, MIN(`t611`.`movie_title`) AS `movie_title`, MIN(`t611`.`movie_year`) AS `movie_year`  FROM (SELECT `t607`.`movie_id`, `t608`.`movie_id` AS `movie_id0`, MIN(`t607`.`production_note`) AS `production_note`  FROM (SELECT `t604`.`id` AS `id0`, `t606`.`movie_id`, MIN(`t606`.`production_note`) AS `production_note`  FROM (SELECT `id`  FROM `company_type`  WHERE `kind` = 'production companies'  GROUP BY `id`) AS `t602`  CROSS JOIN (SELECT `id`  FROM `info_type`  WHERE `info` = 'bottom 10 rank'  GROUP BY `id`) AS `t604`  INNER JOIN (SELECT `movie_id`, `company_type_id`, MIN(`note`) AS `production_note`  FROM `movie_companies`  WHERE `note` NOT LIKE '%(as Metro-Goldwyn-Mayer Pictures)%'  GROUP BY `movie_id`, `company_type_id`) AS `t606` ON `t602`.`id` = `t606`.`company_type_id`  GROUP BY `t604`.`id`, `t606`.`movie_id`) AS `t607`  INNER JOIN (SELECT `movie_id`, `info_type_id`  FROM `movie_info_idx`  GROUP BY `movie_id`, `info_type_id`) AS `t608` ON `t607`.`movie_id` = `t608`.`movie_id` AND `t607`.`id0` = `t608`.`info_type_id`  GROUP BY `t607`.`movie_id`, `t608`.`movie_id`) AS `t609`  INNER JOIN (SELECT `id`, MIN(`title`) AS `movie_title`, MIN(`production_year`) AS `movie_year`  FROM `title`  WHERE `production_year` &gt;= 2005 AND `production_year` &lt;= 2010  GROUP BY `id`) AS `t611` ON `t609`.`movie_id` = `t611`.`id` AND `t609`.`movie_id0` = `t611`.`id`;</t>
-        </is>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>215.13211703300479</v>
+      </c>
+      <c r="B3">
+        <v>250.7287132740021</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1107.209614515305</v>
+      </c>
+      <c r="B4">
+        <v>1127.3357715606689</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0.40554404258728027</v>
+      </c>
+      <c r="B5">
+        <v>1.796159029006958</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0.2403714656829834</v>
+      </c>
+      <c r="B6">
+        <v>1.075284957885742</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>